<commit_message>
Update: updated for version 1.4
</commit_message>
<xml_diff>
--- a/uploads/xlsx/Timetable SE Department (Fall-25) Version-1.4.xlsx
+++ b/uploads/xlsx/Timetable SE Department (Fall-25) Version-1.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zPythonStuff\Superior Academic Tool\uploads\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA858BAB-F8C0-4B37-974C-1067D886A64E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FED041-2C84-42C5-B0CC-6A910AD5E412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="577" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -812,46 +812,6 @@
         <family val="1"/>
       </rPr>
       <t>Mr. Hammad Ghulam Mustafa</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Technopreneurship </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-BSSE-5C &amp; BSSE-5D
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mr. Nagesh Kumar </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-Mr. Sohail Irshaad, Mr. Hafiz Ali Ahmed
-Mr. Rafaqat Ali, Mr. Muhammad Aqib </t>
     </r>
   </si>
   <si>
@@ -2595,6 +2555,13 @@
 BSSE-5B
 Mr. Philemon Philip</t>
   </si>
+  <si>
+    <t xml:space="preserve">Technopreneurship 
+BSSE-5C &amp; BSSE-5D
+Mr. Nagesh Kumar 
+Mr. Muhammad Sohail Irshad, Mr. Hafiz Ali Ahmed
+Mr. Rafaqat Ali, Mr. Muhammad Aqib </t>
+  </si>
 </sst>
 </file>
 
@@ -2604,7 +2571,7 @@
     <numFmt numFmtId="164" formatCode="dddd\ m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="mmmm&quot;-&quot;dd&quot;-&quot;yyyy"/>
   </numFmts>
-  <fonts count="47">
+  <fonts count="46">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2723,13 +2690,6 @@
     </font>
     <font>
       <sz val="13"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -4476,13 +4436,13 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4497,16 +4457,16 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4536,7 +4496,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4551,7 +4511,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4590,46 +4550,46 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4638,7 +4598,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4648,19 +4608,19 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
@@ -4671,7 +4631,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4707,7 +4667,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4716,7 +4676,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4740,7 +4700,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="8" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4749,7 +4709,7 @@
     <xf numFmtId="0" fontId="13" fillId="10" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4810,7 +4770,7 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="103" xfId="0" applyFill="1" applyBorder="1"/>
@@ -4826,7 +4786,7 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4845,10 +4805,10 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4869,7 +4829,7 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4884,7 +4844,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4949,175 +4909,124 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="117" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="41" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="40" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="118" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="118" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5126,22 +5035,175 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5150,68 +5212,89 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -5237,211 +5320,88 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5672,8 +5632,8 @@
   <dimension ref="A1:AB999"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H60" sqref="H60"/>
+      <pane ySplit="5" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5698,10 +5658,10 @@
       <c r="D1" s="123"/>
       <c r="E1" s="123"/>
       <c r="F1" s="123"/>
-      <c r="G1" s="307"/>
-      <c r="H1" s="308"/>
-      <c r="I1" s="308"/>
-      <c r="J1" s="309"/>
+      <c r="G1" s="275"/>
+      <c r="H1" s="276"/>
+      <c r="I1" s="276"/>
+      <c r="J1" s="277"/>
       <c r="K1" s="1"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -5722,20 +5682,20 @@
       <c r="AB1" s="3"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A2" s="311" t="s">
+      <c r="A2" s="280" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="312"/>
-      <c r="C2" s="312"/>
-      <c r="D2" s="312"/>
-      <c r="E2" s="312"/>
+      <c r="B2" s="281"/>
+      <c r="C2" s="281"/>
+      <c r="D2" s="281"/>
+      <c r="E2" s="281"/>
       <c r="F2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="301"/>
-      <c r="H2" s="301"/>
-      <c r="I2" s="301"/>
-      <c r="J2" s="310"/>
+      <c r="G2" s="278"/>
+      <c r="H2" s="278"/>
+      <c r="I2" s="278"/>
+      <c r="J2" s="279"/>
       <c r="K2" s="1"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -5756,18 +5716,18 @@
       <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A3" s="313"/>
-      <c r="B3" s="274"/>
-      <c r="C3" s="274"/>
-      <c r="D3" s="274"/>
-      <c r="E3" s="279"/>
+      <c r="A3" s="236"/>
+      <c r="B3" s="282"/>
+      <c r="C3" s="282"/>
+      <c r="D3" s="282"/>
+      <c r="E3" s="283"/>
       <c r="F3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="316"/>
-      <c r="H3" s="264"/>
-      <c r="I3" s="264"/>
-      <c r="J3" s="221"/>
+      <c r="G3" s="285"/>
+      <c r="H3" s="243"/>
+      <c r="I3" s="243"/>
+      <c r="J3" s="247"/>
       <c r="K3" s="4"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -5788,18 +5748,18 @@
       <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="1:28" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A4" s="314"/>
-      <c r="B4" s="315"/>
-      <c r="C4" s="315"/>
-      <c r="D4" s="315"/>
-      <c r="E4" s="315"/>
+      <c r="A4" s="266"/>
+      <c r="B4" s="284"/>
+      <c r="C4" s="284"/>
+      <c r="D4" s="284"/>
+      <c r="E4" s="284"/>
       <c r="F4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="317"/>
-      <c r="H4" s="318"/>
-      <c r="I4" s="318"/>
-      <c r="J4" s="319"/>
+      <c r="G4" s="286"/>
+      <c r="H4" s="287"/>
+      <c r="I4" s="287"/>
+      <c r="J4" s="288"/>
       <c r="K4" s="4"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -5821,10 +5781,10 @@
     </row>
     <row r="5" spans="1:28" ht="27" customHeight="1" thickBot="1">
       <c r="A5" s="124"/>
-      <c r="B5" s="320" t="s">
+      <c r="B5" s="289" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="312"/>
+      <c r="C5" s="281"/>
       <c r="D5" s="141" t="s">
         <v>3</v>
       </c>
@@ -5898,32 +5858,32 @@
       <c r="AB6" s="3"/>
     </row>
     <row r="7" spans="1:28" ht="75" customHeight="1">
-      <c r="A7" s="322" t="s">
+      <c r="A7" s="293" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="256" t="s">
+      <c r="C7" s="299" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="139" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E7" s="139" t="s">
-        <v>168</v>
-      </c>
-      <c r="F7" s="305" t="s">
-        <v>217</v>
-      </c>
-      <c r="G7" s="306"/>
+        <v>167</v>
+      </c>
+      <c r="F7" s="273" t="s">
+        <v>216</v>
+      </c>
+      <c r="G7" s="274"/>
       <c r="H7" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="I7" s="224" t="s">
-        <v>202</v>
-      </c>
-      <c r="J7" s="221"/>
+      <c r="I7" s="255" t="s">
+        <v>201</v>
+      </c>
+      <c r="J7" s="247"/>
       <c r="K7" s="1"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -5944,26 +5904,26 @@
       <c r="AB7" s="3"/>
     </row>
     <row r="8" spans="1:28" ht="60" customHeight="1">
-      <c r="A8" s="313"/>
+      <c r="A8" s="236"/>
       <c r="B8" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="257"/>
-      <c r="D8" s="304" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="227"/>
-      <c r="F8" s="327" t="s">
-        <v>207</v>
-      </c>
-      <c r="G8" s="328"/>
+      <c r="C8" s="291"/>
+      <c r="D8" s="307" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="256"/>
+      <c r="F8" s="271" t="s">
+        <v>206</v>
+      </c>
+      <c r="G8" s="272"/>
       <c r="H8" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="I8" s="334" t="s">
-        <v>180</v>
-      </c>
-      <c r="J8" s="221"/>
+      <c r="I8" s="246" t="s">
+        <v>179</v>
+      </c>
+      <c r="J8" s="247"/>
       <c r="K8" s="5"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -5984,11 +5944,11 @@
       <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28" ht="61.5" customHeight="1" thickBot="1">
-      <c r="A9" s="313"/>
+      <c r="A9" s="236"/>
       <c r="B9" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="257"/>
+      <c r="C9" s="291"/>
       <c r="D9" s="31" t="s">
         <v>65</v>
       </c>
@@ -6021,11 +5981,11 @@
       <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="1:28" ht="67.5" customHeight="1">
-      <c r="A10" s="313"/>
+      <c r="A10" s="236"/>
       <c r="B10" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="321" t="s">
+      <c r="C10" s="290" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="31" t="s">
@@ -6034,14 +5994,14 @@
       <c r="E10" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="228" t="s">
+      <c r="F10" s="229" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="229"/>
-      <c r="H10" s="224" t="s">
+      <c r="G10" s="250"/>
+      <c r="H10" s="255" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="227"/>
+      <c r="I10" s="256"/>
       <c r="J10" s="101"/>
       <c r="K10" s="3"/>
       <c r="L10" s="2"/>
@@ -6063,25 +6023,25 @@
       <c r="AB10" s="3"/>
     </row>
     <row r="11" spans="1:28" ht="47.25">
-      <c r="A11" s="313"/>
+      <c r="A11" s="236"/>
       <c r="B11" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="257"/>
-      <c r="D11" s="303" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="247"/>
+      <c r="C11" s="291"/>
+      <c r="D11" s="305" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="298"/>
       <c r="F11" s="23" t="s">
         <v>58</v>
       </c>
       <c r="G11" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="228" t="s">
+      <c r="H11" s="229" t="s">
         <v>60</v>
       </c>
-      <c r="I11" s="227"/>
+      <c r="I11" s="256"/>
       <c r="J11" s="102"/>
       <c r="K11" s="5"/>
       <c r="L11" s="2"/>
@@ -6103,22 +6063,22 @@
       <c r="AB11" s="3"/>
     </row>
     <row r="12" spans="1:28" ht="87" customHeight="1">
-      <c r="A12" s="313"/>
+      <c r="A12" s="236"/>
       <c r="B12" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="257"/>
-      <c r="D12" s="234" t="s">
-        <v>218</v>
-      </c>
-      <c r="E12" s="227"/>
+      <c r="C12" s="291"/>
+      <c r="D12" s="268" t="s">
+        <v>217</v>
+      </c>
+      <c r="E12" s="256"/>
       <c r="F12" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="224" t="s">
-        <v>97</v>
-      </c>
-      <c r="H12" s="227"/>
+      <c r="G12" s="255" t="s">
+        <v>271</v>
+      </c>
+      <c r="H12" s="256"/>
       <c r="I12" s="23" t="s">
         <v>62</v>
       </c>
@@ -6143,26 +6103,26 @@
       <c r="AB12" s="3"/>
     </row>
     <row r="13" spans="1:28" ht="47.25">
-      <c r="A13" s="313"/>
+      <c r="A13" s="236"/>
       <c r="B13" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="257"/>
+      <c r="C13" s="291"/>
       <c r="D13" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="E13" s="326" t="s">
-        <v>234</v>
-      </c>
-      <c r="F13" s="227"/>
+        <v>168</v>
+      </c>
+      <c r="E13" s="270" t="s">
+        <v>233</v>
+      </c>
+      <c r="F13" s="256"/>
       <c r="G13" s="23" t="s">
         <v>63</v>
       </c>
       <c r="H13" s="188" t="s">
+        <v>251</v>
+      </c>
+      <c r="I13" s="188" t="s">
         <v>252</v>
-      </c>
-      <c r="I13" s="188" t="s">
-        <v>253</v>
       </c>
       <c r="J13" s="63" t="s">
         <v>96</v>
@@ -6187,11 +6147,11 @@
       <c r="AB13" s="3"/>
     </row>
     <row r="14" spans="1:28" ht="26.25" hidden="1" customHeight="1">
-      <c r="A14" s="313"/>
+      <c r="A14" s="236"/>
       <c r="B14" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="257"/>
+      <c r="C14" s="291"/>
       <c r="D14" s="47"/>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
@@ -6219,28 +6179,28 @@
       <c r="AB14" s="3"/>
     </row>
     <row r="15" spans="1:28" ht="63">
-      <c r="A15" s="313"/>
+      <c r="A15" s="236"/>
       <c r="B15" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="257"/>
-      <c r="D15" s="303" t="s">
+      <c r="C15" s="291"/>
+      <c r="D15" s="305" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="247"/>
+      <c r="E15" s="298"/>
       <c r="F15" s="50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G15" s="50" t="s">
         <v>94</v>
       </c>
       <c r="H15" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="I15" s="224" t="s">
-        <v>129</v>
-      </c>
-      <c r="J15" s="221"/>
+        <v>157</v>
+      </c>
+      <c r="I15" s="255" t="s">
+        <v>128</v>
+      </c>
+      <c r="J15" s="247"/>
       <c r="K15" s="5"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -6261,17 +6221,17 @@
       <c r="AB15" s="3"/>
     </row>
     <row r="16" spans="1:28" ht="57.75" customHeight="1">
-      <c r="A16" s="313"/>
+      <c r="A16" s="236"/>
       <c r="B16" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="257"/>
+      <c r="C16" s="291"/>
       <c r="D16" s="48"/>
       <c r="E16" s="36"/>
-      <c r="F16" s="226" t="s">
-        <v>183</v>
-      </c>
-      <c r="G16" s="260"/>
+      <c r="F16" s="306" t="s">
+        <v>182</v>
+      </c>
+      <c r="G16" s="264"/>
       <c r="H16" s="118"/>
       <c r="I16" s="119"/>
       <c r="J16" s="59"/>
@@ -6295,15 +6255,15 @@
       <c r="AB16" s="3"/>
     </row>
     <row r="17" spans="1:28" ht="71.25" customHeight="1">
-      <c r="A17" s="313"/>
+      <c r="A17" s="236"/>
       <c r="B17" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="257"/>
-      <c r="D17" s="225"/>
-      <c r="E17" s="264"/>
-      <c r="F17" s="243"/>
-      <c r="G17" s="231"/>
+      <c r="C17" s="291"/>
+      <c r="D17" s="242"/>
+      <c r="E17" s="243"/>
+      <c r="F17" s="244"/>
+      <c r="G17" s="245"/>
       <c r="H17" s="120"/>
       <c r="I17" s="120"/>
       <c r="J17" s="89"/>
@@ -6327,15 +6287,15 @@
       <c r="AB17" s="3"/>
     </row>
     <row r="18" spans="1:28" ht="64.5" customHeight="1">
-      <c r="A18" s="313"/>
+      <c r="A18" s="236"/>
       <c r="B18" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="257"/>
+      <c r="C18" s="291"/>
       <c r="D18" s="88"/>
       <c r="E18" s="88"/>
-      <c r="F18" s="243"/>
-      <c r="G18" s="231"/>
+      <c r="F18" s="244"/>
+      <c r="G18" s="245"/>
       <c r="H18" s="120"/>
       <c r="I18" s="120"/>
       <c r="J18" s="117"/>
@@ -6359,23 +6319,23 @@
       <c r="AB18" s="3"/>
     </row>
     <row r="19" spans="1:28" ht="60.75" customHeight="1">
-      <c r="A19" s="313"/>
+      <c r="A19" s="236"/>
       <c r="B19" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="257"/>
-      <c r="D19" s="234" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="227"/>
-      <c r="F19" s="300" t="s">
-        <v>216</v>
-      </c>
-      <c r="G19" s="301"/>
-      <c r="H19" s="230" t="s">
-        <v>125</v>
-      </c>
-      <c r="I19" s="231"/>
+      <c r="C19" s="291"/>
+      <c r="D19" s="268" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="256"/>
+      <c r="F19" s="301" t="s">
+        <v>215</v>
+      </c>
+      <c r="G19" s="278"/>
+      <c r="H19" s="300" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" s="245"/>
       <c r="J19" s="89"/>
       <c r="K19" s="5"/>
       <c r="L19" s="2"/>
@@ -6397,25 +6357,25 @@
       <c r="AB19" s="3"/>
     </row>
     <row r="20" spans="1:28" ht="59.25" customHeight="1" thickBot="1">
-      <c r="A20" s="323"/>
+      <c r="A20" s="294"/>
       <c r="B20" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="258"/>
+      <c r="C20" s="292"/>
       <c r="D20" s="302" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="241"/>
+      <c r="F20" s="240" t="s">
         <v>146</v>
       </c>
-      <c r="E20" s="276"/>
-      <c r="F20" s="275" t="s">
+      <c r="G20" s="241"/>
+      <c r="H20" s="303" t="s">
         <v>147</v>
       </c>
-      <c r="G20" s="276"/>
-      <c r="H20" s="288" t="s">
-        <v>148</v>
-      </c>
-      <c r="I20" s="289"/>
+      <c r="I20" s="304"/>
       <c r="J20" s="84" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="2"/>
@@ -6438,10 +6398,10 @@
     </row>
     <row r="21" spans="1:28" ht="20.25" thickBot="1">
       <c r="A21" s="40"/>
-      <c r="B21" s="344" t="s">
+      <c r="B21" s="262" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="255"/>
+      <c r="C21" s="263"/>
       <c r="D21" s="27"/>
       <c r="E21" s="41"/>
       <c r="F21" s="41"/>
@@ -6469,7 +6429,7 @@
       <c r="AB21" s="3"/>
     </row>
     <row r="22" spans="1:28" ht="20.25" thickBot="1">
-      <c r="A22" s="329" t="s">
+      <c r="A22" s="231" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="90" t="s">
@@ -6517,25 +6477,25 @@
       <c r="AB22" s="3"/>
     </row>
     <row r="23" spans="1:28" ht="47.25" customHeight="1">
-      <c r="A23" s="249"/>
+      <c r="A23" s="232"/>
       <c r="B23" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="345" t="s">
+      <c r="C23" s="265" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="336" t="s">
-        <v>199</v>
-      </c>
-      <c r="E23" s="337"/>
-      <c r="F23" s="338" t="s">
-        <v>126</v>
-      </c>
-      <c r="G23" s="337"/>
-      <c r="H23" s="339" t="s">
-        <v>164</v>
-      </c>
-      <c r="I23" s="337"/>
+      <c r="D23" s="251" t="s">
+        <v>198</v>
+      </c>
+      <c r="E23" s="252"/>
+      <c r="F23" s="253" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="252"/>
+      <c r="H23" s="254" t="s">
+        <v>163</v>
+      </c>
+      <c r="I23" s="252"/>
       <c r="J23" s="98" t="s">
         <v>12</v>
       </c>
@@ -6559,23 +6519,23 @@
       <c r="AB23" s="3"/>
     </row>
     <row r="24" spans="1:28" ht="52.5" customHeight="1">
-      <c r="A24" s="249"/>
+      <c r="A24" s="232"/>
       <c r="B24" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="313"/>
-      <c r="D24" s="224" t="s">
-        <v>195</v>
-      </c>
-      <c r="E24" s="227"/>
-      <c r="F24" s="224" t="s">
-        <v>162</v>
-      </c>
-      <c r="G24" s="227"/>
-      <c r="H24" s="224" t="s">
-        <v>105</v>
-      </c>
-      <c r="I24" s="227"/>
+      <c r="C24" s="236"/>
+      <c r="D24" s="255" t="s">
+        <v>194</v>
+      </c>
+      <c r="E24" s="256"/>
+      <c r="F24" s="255" t="s">
+        <v>161</v>
+      </c>
+      <c r="G24" s="256"/>
+      <c r="H24" s="255" t="s">
+        <v>104</v>
+      </c>
+      <c r="I24" s="256"/>
       <c r="J24" s="58" t="s">
         <v>12</v>
       </c>
@@ -6599,26 +6559,26 @@
       <c r="AB24" s="3"/>
     </row>
     <row r="25" spans="1:28" ht="81" customHeight="1" thickBot="1">
-      <c r="A25" s="249"/>
+      <c r="A25" s="232"/>
       <c r="B25" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="314"/>
+      <c r="C25" s="266"/>
       <c r="D25" s="50"/>
       <c r="E25" s="50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F25" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="G25" s="228" t="s">
-        <v>233</v>
-      </c>
-      <c r="H25" s="341"/>
-      <c r="I25" s="342" t="s">
-        <v>173</v>
-      </c>
-      <c r="J25" s="343"/>
+      <c r="G25" s="229" t="s">
+        <v>232</v>
+      </c>
+      <c r="H25" s="259"/>
+      <c r="I25" s="260" t="s">
+        <v>172</v>
+      </c>
+      <c r="J25" s="261"/>
       <c r="K25" s="7"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -6639,27 +6599,27 @@
       <c r="AB25" s="3"/>
     </row>
     <row r="26" spans="1:28" ht="47.25">
-      <c r="A26" s="249"/>
+      <c r="A26" s="232"/>
       <c r="B26" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="330" t="s">
+      <c r="C26" s="234" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="324" t="s">
-        <v>181</v>
-      </c>
-      <c r="E26" s="227"/>
+      <c r="D26" s="267" t="s">
+        <v>180</v>
+      </c>
+      <c r="E26" s="256"/>
       <c r="F26" s="68" t="s">
         <v>58</v>
       </c>
       <c r="G26" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="H26" s="228" t="s">
+      <c r="H26" s="229" t="s">
         <v>67</v>
       </c>
-      <c r="I26" s="227"/>
+      <c r="I26" s="256"/>
       <c r="J26" s="60"/>
       <c r="K26" s="6"/>
       <c r="L26" s="2"/>
@@ -6681,29 +6641,29 @@
       <c r="AB26" s="3"/>
     </row>
     <row r="27" spans="1:28" ht="47.25">
-      <c r="A27" s="249"/>
+      <c r="A27" s="232"/>
       <c r="B27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="291"/>
+      <c r="C27" s="235"/>
       <c r="D27" s="50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E27" s="64" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F27" s="146" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G27" s="146" t="s">
-        <v>159</v>
-      </c>
-      <c r="H27" s="234" t="s">
-        <v>131</v>
-      </c>
-      <c r="I27" s="227"/>
+        <v>158</v>
+      </c>
+      <c r="H27" s="268" t="s">
+        <v>130</v>
+      </c>
+      <c r="I27" s="256"/>
       <c r="J27" s="63" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K27" s="6"/>
       <c r="L27" s="2"/>
@@ -6725,25 +6685,25 @@
       <c r="AB27" s="3"/>
     </row>
     <row r="28" spans="1:28" ht="63">
-      <c r="A28" s="249"/>
+      <c r="A28" s="232"/>
       <c r="B28" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="291"/>
+      <c r="C28" s="235"/>
       <c r="D28" s="104" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E28" s="69" t="s">
-        <v>174</v>
-      </c>
-      <c r="F28" s="296" t="s">
-        <v>200</v>
-      </c>
-      <c r="G28" s="335"/>
-      <c r="H28" s="228" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" s="248" t="s">
+        <v>199</v>
+      </c>
+      <c r="G28" s="249"/>
+      <c r="H28" s="229" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="227"/>
+      <c r="I28" s="256"/>
       <c r="J28" s="89"/>
       <c r="K28" s="6"/>
       <c r="L28" s="2"/>
@@ -6765,28 +6725,28 @@
       <c r="AB28" s="3"/>
     </row>
     <row r="29" spans="1:28" ht="62.25" customHeight="1">
-      <c r="A29" s="249"/>
+      <c r="A29" s="232"/>
       <c r="B29" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="291"/>
+      <c r="C29" s="235"/>
       <c r="D29" s="23" t="s">
         <v>55</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F29" s="50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G29" s="23" t="s">
         <v>63</v>
       </c>
       <c r="H29" s="188" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I29" s="50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J29" s="63" t="s">
         <v>96</v>
@@ -6811,26 +6771,26 @@
       <c r="AB29" s="3"/>
     </row>
     <row r="30" spans="1:28" ht="63">
-      <c r="A30" s="249"/>
+      <c r="A30" s="232"/>
       <c r="B30" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="291"/>
-      <c r="D30" s="340" t="s">
-        <v>221</v>
-      </c>
-      <c r="E30" s="242"/>
-      <c r="F30" s="325" t="s">
-        <v>175</v>
-      </c>
-      <c r="G30" s="227"/>
+      <c r="C30" s="235"/>
+      <c r="D30" s="257" t="s">
+        <v>220</v>
+      </c>
+      <c r="E30" s="258"/>
+      <c r="F30" s="269" t="s">
+        <v>174</v>
+      </c>
+      <c r="G30" s="256"/>
       <c r="H30" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="I30" s="228" t="s">
-        <v>231</v>
-      </c>
-      <c r="J30" s="221"/>
+        <v>157</v>
+      </c>
+      <c r="I30" s="229" t="s">
+        <v>230</v>
+      </c>
+      <c r="J30" s="247"/>
       <c r="K30" s="6"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -6851,19 +6811,19 @@
       <c r="AB30" s="3"/>
     </row>
     <row r="31" spans="1:28" ht="60.75" customHeight="1">
-      <c r="A31" s="249"/>
+      <c r="A31" s="232"/>
       <c r="B31" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="291"/>
+      <c r="C31" s="235"/>
       <c r="D31" s="129"/>
       <c r="E31" s="130"/>
       <c r="F31" s="131"/>
       <c r="G31" s="132"/>
-      <c r="H31" s="340" t="s">
-        <v>213</v>
-      </c>
-      <c r="I31" s="260"/>
+      <c r="H31" s="257" t="s">
+        <v>212</v>
+      </c>
+      <c r="I31" s="264"/>
       <c r="J31" s="60"/>
       <c r="K31" s="6"/>
       <c r="L31" s="2"/>
@@ -6885,11 +6845,11 @@
       <c r="AB31" s="3"/>
     </row>
     <row r="32" spans="1:28" ht="49.5" customHeight="1">
-      <c r="A32" s="249"/>
+      <c r="A32" s="232"/>
       <c r="B32" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="313"/>
+      <c r="C32" s="236"/>
       <c r="D32" s="120"/>
       <c r="E32" s="120"/>
       <c r="F32" s="120"/>
@@ -6917,11 +6877,11 @@
       <c r="AB32" s="3"/>
     </row>
     <row r="33" spans="1:28" ht="54.75" customHeight="1">
-      <c r="A33" s="249"/>
+      <c r="A33" s="232"/>
       <c r="B33" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="331"/>
+      <c r="C33" s="237"/>
       <c r="D33" s="120"/>
       <c r="E33" s="120"/>
       <c r="F33" s="120"/>
@@ -6949,25 +6909,25 @@
       <c r="AB33" s="3"/>
     </row>
     <row r="34" spans="1:28" ht="49.5">
-      <c r="A34" s="249"/>
+      <c r="A34" s="232"/>
       <c r="B34" s="18" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="296" t="s">
-        <v>188</v>
-      </c>
-      <c r="E34" s="229"/>
-      <c r="F34" s="296" t="s">
-        <v>100</v>
-      </c>
-      <c r="G34" s="229"/>
-      <c r="H34" s="296" t="s">
-        <v>209</v>
-      </c>
-      <c r="I34" s="229"/>
+      <c r="D34" s="248" t="s">
+        <v>187</v>
+      </c>
+      <c r="E34" s="250"/>
+      <c r="F34" s="248" t="s">
+        <v>99</v>
+      </c>
+      <c r="G34" s="250"/>
+      <c r="H34" s="248" t="s">
+        <v>208</v>
+      </c>
+      <c r="I34" s="250"/>
       <c r="J34" s="92"/>
       <c r="K34" s="6"/>
       <c r="L34" s="2"/>
@@ -6989,21 +6949,21 @@
       <c r="AB34" s="3"/>
     </row>
     <row r="35" spans="1:28" ht="53.25" thickBot="1">
-      <c r="A35" s="250"/>
+      <c r="A35" s="233"/>
       <c r="B35" s="77" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="136" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="332" t="s">
-        <v>238</v>
-      </c>
-      <c r="E35" s="333"/>
-      <c r="F35" s="275"/>
-      <c r="G35" s="276"/>
+      <c r="D35" s="238" t="s">
+        <v>237</v>
+      </c>
+      <c r="E35" s="239"/>
+      <c r="F35" s="240"/>
+      <c r="G35" s="241"/>
       <c r="H35" s="83" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I35" s="148"/>
       <c r="J35" s="93"/>
@@ -7028,10 +6988,10 @@
     </row>
     <row r="36" spans="1:28" ht="20.25" thickBot="1">
       <c r="A36" s="44"/>
-      <c r="B36" s="278" t="s">
+      <c r="B36" s="320" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="279"/>
+      <c r="C36" s="283"/>
       <c r="D36" s="27"/>
       <c r="E36" s="41"/>
       <c r="F36" s="41"/>
@@ -7059,7 +7019,7 @@
       <c r="AB36" s="3"/>
     </row>
     <row r="37" spans="1:28" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A37" s="290" t="s">
+      <c r="A37" s="309" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="52" t="s">
@@ -7107,11 +7067,11 @@
       <c r="AB37" s="3"/>
     </row>
     <row r="38" spans="1:28" ht="52.5" customHeight="1">
-      <c r="A38" s="291"/>
+      <c r="A38" s="235"/>
       <c r="B38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="280" t="s">
+      <c r="C38" s="321" t="s">
         <v>30</v>
       </c>
       <c r="D38" s="22" t="s">
@@ -7120,14 +7080,14 @@
       <c r="E38" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="228" t="s">
-        <v>128</v>
-      </c>
-      <c r="G38" s="227"/>
-      <c r="H38" s="224" t="s">
-        <v>160</v>
-      </c>
-      <c r="I38" s="227"/>
+      <c r="F38" s="229" t="s">
+        <v>127</v>
+      </c>
+      <c r="G38" s="256"/>
+      <c r="H38" s="255" t="s">
+        <v>159</v>
+      </c>
+      <c r="I38" s="256"/>
       <c r="J38" s="58" t="s">
         <v>12</v>
       </c>
@@ -7151,23 +7111,23 @@
       <c r="AB38" s="3"/>
     </row>
     <row r="39" spans="1:28" ht="58.5" customHeight="1">
-      <c r="A39" s="291"/>
+      <c r="A39" s="235"/>
       <c r="B39" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="281"/>
-      <c r="D39" s="224" t="s">
-        <v>161</v>
-      </c>
-      <c r="E39" s="229"/>
-      <c r="F39" s="226" t="s">
-        <v>203</v>
-      </c>
-      <c r="G39" s="227"/>
-      <c r="H39" s="228" t="s">
-        <v>127</v>
-      </c>
-      <c r="I39" s="227"/>
+      <c r="C39" s="322"/>
+      <c r="D39" s="255" t="s">
+        <v>160</v>
+      </c>
+      <c r="E39" s="250"/>
+      <c r="F39" s="306" t="s">
+        <v>202</v>
+      </c>
+      <c r="G39" s="256"/>
+      <c r="H39" s="229" t="s">
+        <v>126</v>
+      </c>
+      <c r="I39" s="256"/>
       <c r="J39" s="58" t="s">
         <v>12</v>
       </c>
@@ -7191,15 +7151,15 @@
       <c r="AB39" s="3"/>
     </row>
     <row r="40" spans="1:28" ht="57" customHeight="1">
-      <c r="A40" s="291"/>
+      <c r="A40" s="235"/>
       <c r="B40" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="282"/>
-      <c r="D40" s="224" t="s">
-        <v>112</v>
-      </c>
-      <c r="E40" s="264"/>
+      <c r="C40" s="323"/>
+      <c r="D40" s="255" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" s="243"/>
       <c r="F40" s="120"/>
       <c r="G40" s="88"/>
       <c r="H40" s="22" t="s">
@@ -7231,28 +7191,28 @@
       <c r="AB40" s="3"/>
     </row>
     <row r="41" spans="1:28" ht="55.5" customHeight="1">
-      <c r="A41" s="291"/>
+      <c r="A41" s="235"/>
       <c r="B41" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="283" t="s">
+      <c r="C41" s="324" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="224" t="s">
+      <c r="D41" s="255" t="s">
         <v>69</v>
       </c>
-      <c r="E41" s="247"/>
-      <c r="F41" s="241" t="s">
+      <c r="E41" s="298"/>
+      <c r="F41" s="353" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="242"/>
+      <c r="G41" s="258"/>
       <c r="H41" s="190" t="s">
-        <v>253</v>
-      </c>
-      <c r="I41" s="234" t="s">
+        <v>252</v>
+      </c>
+      <c r="I41" s="268" t="s">
         <v>85</v>
       </c>
-      <c r="J41" s="235"/>
+      <c r="J41" s="347"/>
       <c r="K41" s="6"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
@@ -7273,26 +7233,26 @@
       <c r="AB41" s="3"/>
     </row>
     <row r="42" spans="1:28" ht="64.5" customHeight="1">
-      <c r="A42" s="291"/>
+      <c r="A42" s="235"/>
       <c r="B42" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="281"/>
-      <c r="D42" s="224" t="s">
-        <v>155</v>
-      </c>
-      <c r="E42" s="264"/>
+      <c r="C42" s="322"/>
+      <c r="D42" s="255" t="s">
+        <v>154</v>
+      </c>
+      <c r="E42" s="243"/>
       <c r="F42" s="146" t="s">
         <v>72</v>
       </c>
       <c r="G42" s="146" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H42" s="67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I42" s="50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J42" s="191"/>
       <c r="K42" s="6"/>
@@ -7315,22 +7275,22 @@
       <c r="AB42" s="3"/>
     </row>
     <row r="43" spans="1:28" ht="108.75" customHeight="1">
-      <c r="A43" s="291"/>
+      <c r="A43" s="235"/>
       <c r="B43" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="281"/>
-      <c r="D43" s="228" t="s">
-        <v>219</v>
-      </c>
-      <c r="E43" s="247"/>
+      <c r="C43" s="322"/>
+      <c r="D43" s="229" t="s">
+        <v>218</v>
+      </c>
+      <c r="E43" s="298"/>
       <c r="F43" s="139" t="s">
-        <v>201</v>
-      </c>
-      <c r="G43" s="296" t="s">
-        <v>258</v>
-      </c>
-      <c r="H43" s="227"/>
+        <v>200</v>
+      </c>
+      <c r="G43" s="248" t="s">
+        <v>257</v>
+      </c>
+      <c r="H43" s="256"/>
       <c r="I43" s="88"/>
       <c r="J43" s="89"/>
       <c r="K43" s="6"/>
@@ -7353,22 +7313,22 @@
       <c r="AB43" s="3"/>
     </row>
     <row r="44" spans="1:28" ht="63" customHeight="1">
-      <c r="A44" s="291"/>
+      <c r="A44" s="235"/>
       <c r="B44" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="281"/>
-      <c r="D44" s="245" t="s">
-        <v>235</v>
-      </c>
-      <c r="E44" s="246"/>
+      <c r="C44" s="322"/>
+      <c r="D44" s="354" t="s">
+        <v>234</v>
+      </c>
+      <c r="E44" s="355"/>
       <c r="F44" s="23" t="s">
-        <v>208</v>
-      </c>
-      <c r="G44" s="224" t="s">
+        <v>207</v>
+      </c>
+      <c r="G44" s="255" t="s">
         <v>87</v>
       </c>
-      <c r="H44" s="227"/>
+      <c r="H44" s="256"/>
       <c r="I44" s="26"/>
       <c r="J44" s="60"/>
       <c r="K44" s="6"/>
@@ -7391,13 +7351,13 @@
       <c r="AB44" s="3"/>
     </row>
     <row r="45" spans="1:28" ht="64.5" hidden="1" customHeight="1">
-      <c r="A45" s="291"/>
+      <c r="A45" s="235"/>
       <c r="B45" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="281"/>
-      <c r="D45" s="297"/>
-      <c r="E45" s="227"/>
+      <c r="C45" s="322"/>
+      <c r="D45" s="314"/>
+      <c r="E45" s="256"/>
       <c r="F45" s="26"/>
       <c r="G45" s="38"/>
       <c r="H45" s="26"/>
@@ -7423,11 +7383,11 @@
       <c r="AB45" s="3"/>
     </row>
     <row r="46" spans="1:28" ht="47.25">
-      <c r="A46" s="291"/>
+      <c r="A46" s="235"/>
       <c r="B46" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="281"/>
+      <c r="C46" s="322"/>
       <c r="D46" s="189" t="s">
         <v>73</v>
       </c>
@@ -7435,15 +7395,15 @@
         <v>74</v>
       </c>
       <c r="F46" s="85" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G46" s="85" t="s">
-        <v>136</v>
-      </c>
-      <c r="H46" s="224" t="s">
-        <v>153</v>
-      </c>
-      <c r="I46" s="227"/>
+        <v>135</v>
+      </c>
+      <c r="H46" s="255" t="s">
+        <v>152</v>
+      </c>
+      <c r="I46" s="256"/>
       <c r="J46" s="63" t="s">
         <v>32</v>
       </c>
@@ -7467,19 +7427,19 @@
       <c r="AB46" s="3"/>
     </row>
     <row r="47" spans="1:28" ht="50.25" customHeight="1">
-      <c r="A47" s="291"/>
+      <c r="A47" s="235"/>
       <c r="B47" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="281"/>
+      <c r="C47" s="322"/>
       <c r="D47" s="129"/>
       <c r="E47" s="130"/>
       <c r="F47" s="131"/>
       <c r="G47" s="132"/>
-      <c r="H47" s="226" t="s">
-        <v>154</v>
-      </c>
-      <c r="I47" s="260"/>
+      <c r="H47" s="306" t="s">
+        <v>153</v>
+      </c>
+      <c r="I47" s="264"/>
       <c r="J47" s="59"/>
       <c r="K47" s="6"/>
       <c r="L47" s="2"/>
@@ -7501,11 +7461,11 @@
       <c r="AB47" s="3"/>
     </row>
     <row r="48" spans="1:28" ht="49.5" customHeight="1">
-      <c r="A48" s="291"/>
+      <c r="A48" s="235"/>
       <c r="B48" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="284"/>
+      <c r="C48" s="325"/>
       <c r="D48" s="120"/>
       <c r="E48" s="120"/>
       <c r="F48" s="120"/>
@@ -7533,15 +7493,15 @@
       <c r="AB48" s="3"/>
     </row>
     <row r="49" spans="1:28" ht="53.25" customHeight="1">
-      <c r="A49" s="291"/>
+      <c r="A49" s="235"/>
       <c r="B49" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C49" s="285"/>
-      <c r="D49" s="243" t="s">
-        <v>104</v>
-      </c>
-      <c r="E49" s="231"/>
+      <c r="C49" s="326"/>
+      <c r="D49" s="244" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" s="245"/>
       <c r="F49" s="120"/>
       <c r="G49" s="120"/>
       <c r="H49" s="120"/>
@@ -7567,7 +7527,7 @@
       <c r="AB49" s="3"/>
     </row>
     <row r="50" spans="1:28" ht="49.5">
-      <c r="A50" s="291"/>
+      <c r="A50" s="235"/>
       <c r="B50" s="19" t="s">
         <v>25</v>
       </c>
@@ -7575,17 +7535,17 @@
         <v>11</v>
       </c>
       <c r="D50" s="147" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E50" s="140"/>
-      <c r="F50" s="230" t="s">
-        <v>223</v>
-      </c>
-      <c r="G50" s="231"/>
-      <c r="H50" s="230" t="s">
-        <v>197</v>
-      </c>
-      <c r="I50" s="231"/>
+      <c r="F50" s="300" t="s">
+        <v>222</v>
+      </c>
+      <c r="G50" s="245"/>
+      <c r="H50" s="300" t="s">
+        <v>196</v>
+      </c>
+      <c r="I50" s="245"/>
       <c r="J50" s="117"/>
       <c r="K50" s="8"/>
       <c r="L50" s="2"/>
@@ -7607,7 +7567,7 @@
       <c r="AB50" s="3"/>
     </row>
     <row r="51" spans="1:28" ht="79.5" thickBot="1">
-      <c r="A51" s="292"/>
+      <c r="A51" s="310"/>
       <c r="B51" s="61" t="s">
         <v>26</v>
       </c>
@@ -7620,16 +7580,16 @@
       <c r="E51" s="138" t="s">
         <v>76</v>
       </c>
-      <c r="F51" s="236" t="s">
-        <v>225</v>
-      </c>
-      <c r="G51" s="237"/>
-      <c r="H51" s="288" t="s">
+      <c r="F51" s="348" t="s">
+        <v>224</v>
+      </c>
+      <c r="G51" s="349"/>
+      <c r="H51" s="303" t="s">
+        <v>148</v>
+      </c>
+      <c r="I51" s="304"/>
+      <c r="J51" s="84" t="s">
         <v>149</v>
-      </c>
-      <c r="I51" s="289"/>
-      <c r="J51" s="84" t="s">
-        <v>150</v>
       </c>
       <c r="K51" s="82"/>
       <c r="L51" s="9"/>
@@ -7652,10 +7612,10 @@
     </row>
     <row r="52" spans="1:28" ht="21.75" customHeight="1" thickBot="1">
       <c r="A52" s="45"/>
-      <c r="B52" s="286" t="s">
+      <c r="B52" s="327" t="s">
         <v>33</v>
       </c>
-      <c r="C52" s="255"/>
+      <c r="C52" s="263"/>
       <c r="D52" s="27"/>
       <c r="E52" s="28"/>
       <c r="F52" s="28"/>
@@ -7683,7 +7643,7 @@
       <c r="AB52" s="3"/>
     </row>
     <row r="53" spans="1:28" ht="19.5">
-      <c r="A53" s="293" t="s">
+      <c r="A53" s="311" t="s">
         <v>33</v>
       </c>
       <c r="B53" s="155" t="s">
@@ -7731,25 +7691,25 @@
       <c r="AB53" s="3"/>
     </row>
     <row r="54" spans="1:28" ht="56.25" customHeight="1">
-      <c r="A54" s="294"/>
+      <c r="A54" s="312"/>
       <c r="B54" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="C54" s="251" t="s">
+      <c r="C54" s="330" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="243" t="s">
-        <v>165</v>
-      </c>
-      <c r="E54" s="231"/>
-      <c r="F54" s="243" t="s">
-        <v>163</v>
-      </c>
-      <c r="G54" s="231"/>
-      <c r="H54" s="243" t="s">
-        <v>205</v>
-      </c>
-      <c r="I54" s="231"/>
+      <c r="D54" s="244" t="s">
+        <v>164</v>
+      </c>
+      <c r="E54" s="245"/>
+      <c r="F54" s="244" t="s">
+        <v>162</v>
+      </c>
+      <c r="G54" s="245"/>
+      <c r="H54" s="244" t="s">
+        <v>204</v>
+      </c>
+      <c r="I54" s="245"/>
       <c r="J54" s="159" t="s">
         <v>12</v>
       </c>
@@ -7773,24 +7733,24 @@
       <c r="AB54" s="3"/>
     </row>
     <row r="55" spans="1:28" ht="60" customHeight="1">
-      <c r="A55" s="294"/>
+      <c r="A55" s="312"/>
       <c r="B55" s="150" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="231"/>
-      <c r="D55" s="243" t="s">
+      <c r="C55" s="245"/>
+      <c r="D55" s="244" t="s">
+        <v>141</v>
+      </c>
+      <c r="E55" s="245"/>
+      <c r="F55" s="244" t="s">
         <v>142</v>
       </c>
-      <c r="E55" s="231"/>
-      <c r="F55" s="243" t="s">
-        <v>143</v>
-      </c>
-      <c r="G55" s="231"/>
+      <c r="G55" s="245"/>
       <c r="H55" s="151" t="s">
         <v>12</v>
       </c>
-      <c r="I55" s="222"/>
-      <c r="J55" s="223"/>
+      <c r="I55" s="345"/>
+      <c r="J55" s="346"/>
       <c r="K55" s="5"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
@@ -7811,28 +7771,28 @@
       <c r="AB55" s="3"/>
     </row>
     <row r="56" spans="1:28" ht="78" customHeight="1">
-      <c r="A56" s="294"/>
+      <c r="A56" s="312"/>
       <c r="B56" s="150" t="s">
         <v>14</v>
       </c>
-      <c r="C56" s="231"/>
+      <c r="C56" s="245"/>
       <c r="D56" s="151" t="s">
         <v>12</v>
       </c>
       <c r="E56" s="151" t="s">
         <v>12</v>
       </c>
-      <c r="F56" s="230" t="s">
-        <v>130</v>
-      </c>
-      <c r="G56" s="231"/>
+      <c r="F56" s="300" t="s">
+        <v>129</v>
+      </c>
+      <c r="G56" s="245"/>
       <c r="H56" s="146" t="s">
         <v>77</v>
       </c>
-      <c r="I56" s="243" t="s">
-        <v>151</v>
-      </c>
-      <c r="J56" s="244"/>
+      <c r="I56" s="244" t="s">
+        <v>150</v>
+      </c>
+      <c r="J56" s="308"/>
       <c r="K56" s="6"/>
       <c r="L56" s="2"/>
       <c r="M56" s="2"/>
@@ -7853,21 +7813,21 @@
       <c r="AB56" s="3"/>
     </row>
     <row r="57" spans="1:28" ht="47.25">
-      <c r="A57" s="294"/>
+      <c r="A57" s="312"/>
       <c r="B57" s="150" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="252" t="s">
+      <c r="C57" s="331" t="s">
         <v>16</v>
       </c>
-      <c r="D57" s="232" t="s">
-        <v>236</v>
-      </c>
-      <c r="E57" s="233"/>
-      <c r="F57" s="238" t="s">
-        <v>227</v>
-      </c>
-      <c r="G57" s="238"/>
+      <c r="D57" s="315" t="s">
+        <v>235</v>
+      </c>
+      <c r="E57" s="316"/>
+      <c r="F57" s="350" t="s">
+        <v>226</v>
+      </c>
+      <c r="G57" s="350"/>
       <c r="H57" s="146" t="s">
         <v>75</v>
       </c>
@@ -7895,27 +7855,27 @@
       <c r="AB57" s="3"/>
     </row>
     <row r="58" spans="1:28" ht="60" customHeight="1">
-      <c r="A58" s="294"/>
+      <c r="A58" s="312"/>
       <c r="B58" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="C58" s="231"/>
+      <c r="C58" s="245"/>
       <c r="D58" s="152" t="s">
+        <v>136</v>
+      </c>
+      <c r="E58" s="152" t="s">
         <v>137</v>
       </c>
-      <c r="E58" s="152" t="s">
-        <v>138</v>
-      </c>
       <c r="F58" s="145" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G58" s="146" t="s">
-        <v>224</v>
-      </c>
-      <c r="H58" s="230" t="s">
+        <v>223</v>
+      </c>
+      <c r="H58" s="300" t="s">
         <v>71</v>
       </c>
-      <c r="I58" s="230"/>
+      <c r="I58" s="300"/>
       <c r="J58" s="161"/>
       <c r="K58" s="5"/>
       <c r="L58" s="2"/>
@@ -7937,26 +7897,26 @@
       <c r="AB58" s="3"/>
     </row>
     <row r="59" spans="1:28" ht="54" customHeight="1">
-      <c r="A59" s="294"/>
+      <c r="A59" s="312"/>
       <c r="B59" s="150" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="231"/>
-      <c r="D59" s="243" t="s">
+      <c r="C59" s="245"/>
+      <c r="D59" s="244" t="s">
         <v>78</v>
       </c>
-      <c r="E59" s="231"/>
+      <c r="E59" s="245"/>
       <c r="F59" s="146" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G59" s="146" t="s">
         <v>61</v>
       </c>
       <c r="H59" s="149" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I59" s="149" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J59" s="161"/>
       <c r="K59" s="5"/>
@@ -7979,15 +7939,15 @@
       <c r="AB59" s="3"/>
     </row>
     <row r="60" spans="1:28" ht="53.25" customHeight="1">
-      <c r="A60" s="294"/>
+      <c r="A60" s="312"/>
       <c r="B60" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="C60" s="231"/>
-      <c r="D60" s="243" t="s">
+      <c r="C60" s="245"/>
+      <c r="D60" s="244" t="s">
         <v>88</v>
       </c>
-      <c r="E60" s="231"/>
+      <c r="E60" s="245"/>
       <c r="F60" s="145" t="s">
         <v>90</v>
       </c>
@@ -7995,7 +7955,7 @@
         <v>91</v>
       </c>
       <c r="H60" s="145" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I60" s="146" t="s">
         <v>79</v>
@@ -8021,26 +7981,26 @@
       <c r="AB60" s="3"/>
     </row>
     <row r="61" spans="1:28" ht="47.25">
-      <c r="A61" s="294"/>
+      <c r="A61" s="312"/>
       <c r="B61" s="150" t="s">
         <v>21</v>
       </c>
-      <c r="C61" s="231"/>
+      <c r="C61" s="245"/>
       <c r="D61" s="120"/>
       <c r="E61" s="120"/>
       <c r="F61" s="152" t="s">
+        <v>138</v>
+      </c>
+      <c r="G61" s="152" t="s">
         <v>139</v>
       </c>
-      <c r="G61" s="152" t="s">
-        <v>140</v>
-      </c>
       <c r="H61" s="145" t="s">
-        <v>170</v>
-      </c>
-      <c r="I61" s="230" t="s">
-        <v>232</v>
-      </c>
-      <c r="J61" s="244"/>
+        <v>169</v>
+      </c>
+      <c r="I61" s="300" t="s">
+        <v>231</v>
+      </c>
+      <c r="J61" s="308"/>
       <c r="K61" s="5"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
@@ -8061,21 +8021,21 @@
       <c r="AB61" s="3"/>
     </row>
     <row r="62" spans="1:28" ht="47.25" customHeight="1">
-      <c r="A62" s="294"/>
+      <c r="A62" s="312"/>
       <c r="B62" s="150" t="s">
         <v>22</v>
       </c>
-      <c r="C62" s="231"/>
+      <c r="C62" s="245"/>
       <c r="D62" s="153"/>
       <c r="E62" s="153"/>
-      <c r="F62" s="243" t="s">
-        <v>152</v>
-      </c>
-      <c r="G62" s="231"/>
-      <c r="H62" s="232" t="s">
-        <v>156</v>
-      </c>
-      <c r="I62" s="233"/>
+      <c r="F62" s="244" t="s">
+        <v>151</v>
+      </c>
+      <c r="G62" s="245"/>
+      <c r="H62" s="315" t="s">
+        <v>155</v>
+      </c>
+      <c r="I62" s="316"/>
       <c r="J62" s="162"/>
       <c r="K62" s="5"/>
       <c r="L62" s="2"/>
@@ -8097,11 +8057,11 @@
       <c r="AB62" s="3"/>
     </row>
     <row r="63" spans="1:28" ht="53.25" customHeight="1">
-      <c r="A63" s="294"/>
+      <c r="A63" s="312"/>
       <c r="B63" s="150" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="253" t="s">
+      <c r="C63" s="332" t="s">
         <v>16</v>
       </c>
       <c r="D63" s="120"/>
@@ -8131,19 +8091,19 @@
       <c r="AB63" s="3"/>
     </row>
     <row r="64" spans="1:28" ht="51" customHeight="1">
-      <c r="A64" s="294"/>
+      <c r="A64" s="312"/>
       <c r="B64" s="150" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="231"/>
+      <c r="C64" s="245"/>
       <c r="D64" s="120"/>
       <c r="E64" s="120"/>
       <c r="F64" s="120"/>
       <c r="G64" s="120"/>
-      <c r="H64" s="243" t="s">
-        <v>166</v>
-      </c>
-      <c r="I64" s="231"/>
+      <c r="H64" s="244" t="s">
+        <v>165</v>
+      </c>
+      <c r="I64" s="245"/>
       <c r="J64" s="162"/>
       <c r="K64" s="5"/>
       <c r="L64" s="2"/>
@@ -8165,7 +8125,7 @@
       <c r="AB64" s="3"/>
     </row>
     <row r="65" spans="1:28" ht="50.25" customHeight="1">
-      <c r="A65" s="294"/>
+      <c r="A65" s="312"/>
       <c r="B65" s="150" t="s">
         <v>25</v>
       </c>
@@ -8173,19 +8133,19 @@
         <v>34</v>
       </c>
       <c r="D65" s="145" t="s">
+        <v>143</v>
+      </c>
+      <c r="E65" s="145" t="s">
         <v>144</v>
       </c>
-      <c r="E65" s="145" t="s">
-        <v>145</v>
-      </c>
-      <c r="F65" s="243" t="s">
-        <v>157</v>
-      </c>
-      <c r="G65" s="231"/>
-      <c r="H65" s="243" t="s">
-        <v>204</v>
-      </c>
-      <c r="I65" s="231"/>
+      <c r="F65" s="244" t="s">
+        <v>156</v>
+      </c>
+      <c r="G65" s="245"/>
+      <c r="H65" s="244" t="s">
+        <v>203</v>
+      </c>
+      <c r="I65" s="245"/>
       <c r="J65" s="161"/>
       <c r="K65" s="5"/>
       <c r="L65" s="2"/>
@@ -8207,7 +8167,7 @@
       <c r="AB65" s="3"/>
     </row>
     <row r="66" spans="1:28" ht="66.75" customHeight="1" thickBot="1">
-      <c r="A66" s="295"/>
+      <c r="A66" s="313"/>
       <c r="B66" s="163" t="s">
         <v>26</v>
       </c>
@@ -8216,16 +8176,16 @@
       </c>
       <c r="D66" s="165"/>
       <c r="E66" s="166" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F66" s="167" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G66" s="167" t="s">
         <v>72</v>
       </c>
       <c r="H66" s="167" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I66" s="176"/>
       <c r="J66" s="168"/>
@@ -8250,10 +8210,10 @@
     </row>
     <row r="67" spans="1:28" ht="20.25" thickBot="1">
       <c r="A67" s="45"/>
-      <c r="B67" s="254" t="s">
+      <c r="B67" s="333" t="s">
         <v>35</v>
       </c>
-      <c r="C67" s="255"/>
+      <c r="C67" s="263"/>
       <c r="D67" s="27"/>
       <c r="E67" s="32"/>
       <c r="F67" s="32"/>
@@ -8281,7 +8241,7 @@
       <c r="AB67" s="3"/>
     </row>
     <row r="68" spans="1:28" ht="61.5" customHeight="1" thickBot="1">
-      <c r="A68" s="248" t="s">
+      <c r="A68" s="329" t="s">
         <v>36</v>
       </c>
       <c r="B68" s="70" t="s">
@@ -8327,11 +8287,11 @@
       <c r="AB68" s="3"/>
     </row>
     <row r="69" spans="1:28" ht="64.5" customHeight="1">
-      <c r="A69" s="249"/>
+      <c r="A69" s="232"/>
       <c r="B69" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C69" s="256" t="s">
+      <c r="C69" s="299" t="s">
         <v>43</v>
       </c>
       <c r="D69" s="46" t="s">
@@ -8346,8 +8306,8 @@
       <c r="G69" s="178" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="261" t="s">
-        <v>172</v>
+      <c r="H69" s="335" t="s">
+        <v>171</v>
       </c>
       <c r="I69" s="46" t="s">
         <v>12</v>
@@ -8375,26 +8335,26 @@
       <c r="AB69" s="3"/>
     </row>
     <row r="70" spans="1:28" ht="50.25" customHeight="1">
-      <c r="A70" s="249"/>
+      <c r="A70" s="232"/>
       <c r="B70" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C70" s="257"/>
+      <c r="C70" s="291"/>
       <c r="D70" s="46" t="s">
         <v>12</v>
       </c>
       <c r="E70" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F70" s="224" t="s">
+      <c r="F70" s="255" t="s">
         <v>89</v>
       </c>
-      <c r="G70" s="225"/>
-      <c r="H70" s="257"/>
-      <c r="I70" s="239" t="s">
-        <v>228</v>
-      </c>
-      <c r="J70" s="240"/>
+      <c r="G70" s="242"/>
+      <c r="H70" s="291"/>
+      <c r="I70" s="351" t="s">
+        <v>227</v>
+      </c>
+      <c r="J70" s="352"/>
       <c r="K70" s="6"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
@@ -8415,24 +8375,24 @@
       <c r="AB70" s="3"/>
     </row>
     <row r="71" spans="1:28" ht="52.5" customHeight="1" thickBot="1">
-      <c r="A71" s="249"/>
+      <c r="A71" s="232"/>
       <c r="B71" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C71" s="258"/>
-      <c r="D71" s="262" t="s">
-        <v>189</v>
-      </c>
-      <c r="E71" s="263"/>
+      <c r="C71" s="292"/>
+      <c r="D71" s="336" t="s">
+        <v>188</v>
+      </c>
+      <c r="E71" s="337"/>
       <c r="F71" s="50"/>
       <c r="G71" s="177" t="s">
-        <v>132</v>
-      </c>
-      <c r="H71" s="257"/>
-      <c r="I71" s="220" t="s">
-        <v>190</v>
-      </c>
-      <c r="J71" s="221"/>
+        <v>131</v>
+      </c>
+      <c r="H71" s="291"/>
+      <c r="I71" s="338" t="s">
+        <v>189</v>
+      </c>
+      <c r="J71" s="247"/>
       <c r="K71" s="6"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
@@ -8453,26 +8413,26 @@
       <c r="AB71" s="3"/>
     </row>
     <row r="72" spans="1:28" ht="52.5" customHeight="1">
-      <c r="A72" s="249"/>
+      <c r="A72" s="232"/>
       <c r="B72" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C72" s="259" t="s">
+      <c r="C72" s="334" t="s">
         <v>16</v>
       </c>
-      <c r="D72" s="262" t="s">
+      <c r="D72" s="336" t="s">
         <v>80</v>
       </c>
-      <c r="E72" s="263"/>
-      <c r="F72" s="224" t="s">
-        <v>179</v>
-      </c>
-      <c r="G72" s="264"/>
-      <c r="H72" s="257"/>
-      <c r="I72" s="220" t="s">
+      <c r="E72" s="337"/>
+      <c r="F72" s="255" t="s">
+        <v>178</v>
+      </c>
+      <c r="G72" s="243"/>
+      <c r="H72" s="291"/>
+      <c r="I72" s="338" t="s">
         <v>81</v>
       </c>
-      <c r="J72" s="221"/>
+      <c r="J72" s="247"/>
       <c r="K72" s="6"/>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
@@ -8493,26 +8453,26 @@
       <c r="AB72" s="3"/>
     </row>
     <row r="73" spans="1:28" ht="61.5" customHeight="1">
-      <c r="A73" s="249"/>
+      <c r="A73" s="232"/>
       <c r="B73" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C73" s="257"/>
+      <c r="C73" s="291"/>
       <c r="D73" s="87" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E73" s="86" t="s">
-        <v>138</v>
-      </c>
-      <c r="F73" s="265" t="s">
+        <v>137</v>
+      </c>
+      <c r="F73" s="339" t="s">
+        <v>254</v>
+      </c>
+      <c r="G73" s="297"/>
+      <c r="H73" s="291"/>
+      <c r="I73" s="340" t="s">
         <v>255</v>
       </c>
-      <c r="G73" s="266"/>
-      <c r="H73" s="257"/>
-      <c r="I73" s="267" t="s">
-        <v>256</v>
-      </c>
-      <c r="J73" s="268"/>
+      <c r="J73" s="341"/>
       <c r="K73" s="6"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
@@ -8533,24 +8493,24 @@
       <c r="AB73" s="3"/>
     </row>
     <row r="74" spans="1:28" ht="60.75" customHeight="1">
-      <c r="A74" s="249"/>
+      <c r="A74" s="232"/>
       <c r="B74" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C74" s="257"/>
-      <c r="D74" s="234" t="s">
-        <v>167</v>
-      </c>
-      <c r="E74" s="227"/>
-      <c r="F74" s="287" t="s">
+      <c r="C74" s="291"/>
+      <c r="D74" s="268" t="s">
+        <v>166</v>
+      </c>
+      <c r="E74" s="256"/>
+      <c r="F74" s="328" t="s">
+        <v>113</v>
+      </c>
+      <c r="G74" s="243"/>
+      <c r="H74" s="291"/>
+      <c r="I74" s="295" t="s">
         <v>114</v>
       </c>
-      <c r="G74" s="264"/>
-      <c r="H74" s="257"/>
-      <c r="I74" s="298" t="s">
-        <v>115</v>
-      </c>
-      <c r="J74" s="221"/>
+      <c r="J74" s="247"/>
       <c r="K74" s="6"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
@@ -8571,24 +8531,24 @@
       <c r="AB74" s="3"/>
     </row>
     <row r="75" spans="1:28" ht="69" customHeight="1">
-      <c r="A75" s="249"/>
+      <c r="A75" s="232"/>
       <c r="B75" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C75" s="257"/>
-      <c r="D75" s="234" t="s">
+      <c r="C75" s="291"/>
+      <c r="D75" s="268" t="s">
         <v>82</v>
       </c>
-      <c r="E75" s="227"/>
-      <c r="F75" s="225" t="s">
-        <v>122</v>
-      </c>
-      <c r="G75" s="264"/>
-      <c r="H75" s="257"/>
-      <c r="I75" s="225" t="s">
-        <v>113</v>
-      </c>
-      <c r="J75" s="221"/>
+      <c r="E75" s="256"/>
+      <c r="F75" s="242" t="s">
+        <v>121</v>
+      </c>
+      <c r="G75" s="243"/>
+      <c r="H75" s="291"/>
+      <c r="I75" s="242" t="s">
+        <v>112</v>
+      </c>
+      <c r="J75" s="247"/>
       <c r="K75" s="6"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
@@ -8609,24 +8569,24 @@
       <c r="AB75" s="3"/>
     </row>
     <row r="76" spans="1:28" ht="53.25" customHeight="1">
-      <c r="A76" s="249"/>
+      <c r="A76" s="232"/>
       <c r="B76" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C76" s="257"/>
-      <c r="D76" s="224" t="s">
-        <v>184</v>
-      </c>
-      <c r="E76" s="247"/>
-      <c r="F76" s="299" t="s">
-        <v>254</v>
-      </c>
-      <c r="G76" s="266"/>
-      <c r="H76" s="257"/>
-      <c r="I76" s="225" t="s">
-        <v>133</v>
-      </c>
-      <c r="J76" s="221"/>
+      <c r="C76" s="291"/>
+      <c r="D76" s="255" t="s">
+        <v>183</v>
+      </c>
+      <c r="E76" s="298"/>
+      <c r="F76" s="296" t="s">
+        <v>253</v>
+      </c>
+      <c r="G76" s="297"/>
+      <c r="H76" s="291"/>
+      <c r="I76" s="242" t="s">
+        <v>132</v>
+      </c>
+      <c r="J76" s="247"/>
       <c r="K76" s="6"/>
       <c r="L76" s="2"/>
       <c r="M76" s="2"/>
@@ -8647,22 +8607,22 @@
       <c r="AB76" s="3"/>
     </row>
     <row r="77" spans="1:28" ht="57" customHeight="1">
-      <c r="A77" s="249"/>
+      <c r="A77" s="232"/>
       <c r="B77" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C77" s="257"/>
-      <c r="D77" s="228" t="s">
-        <v>230</v>
-      </c>
-      <c r="E77" s="247"/>
+      <c r="C77" s="291"/>
+      <c r="D77" s="229" t="s">
+        <v>229</v>
+      </c>
+      <c r="E77" s="298"/>
       <c r="F77" s="25"/>
       <c r="G77" s="192"/>
-      <c r="H77" s="257"/>
-      <c r="I77" s="234" t="s">
-        <v>229</v>
-      </c>
-      <c r="J77" s="221"/>
+      <c r="H77" s="291"/>
+      <c r="I77" s="268" t="s">
+        <v>228</v>
+      </c>
+      <c r="J77" s="247"/>
       <c r="K77" s="11"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
@@ -8683,24 +8643,24 @@
       <c r="AB77" s="3"/>
     </row>
     <row r="78" spans="1:28" ht="55.5" customHeight="1">
-      <c r="A78" s="249"/>
+      <c r="A78" s="232"/>
       <c r="B78" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C78" s="257"/>
-      <c r="D78" s="234" t="s">
+      <c r="C78" s="291"/>
+      <c r="D78" s="268" t="s">
         <v>83</v>
       </c>
-      <c r="E78" s="227"/>
-      <c r="F78" s="224" t="s">
-        <v>196</v>
-      </c>
-      <c r="G78" s="264"/>
-      <c r="H78" s="257"/>
-      <c r="I78" s="225" t="s">
-        <v>198</v>
-      </c>
-      <c r="J78" s="221"/>
+      <c r="E78" s="256"/>
+      <c r="F78" s="255" t="s">
+        <v>195</v>
+      </c>
+      <c r="G78" s="243"/>
+      <c r="H78" s="291"/>
+      <c r="I78" s="242" t="s">
+        <v>197</v>
+      </c>
+      <c r="J78" s="247"/>
       <c r="K78" s="6"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
@@ -8721,16 +8681,16 @@
       <c r="AB78" s="3"/>
     </row>
     <row r="79" spans="1:28" ht="64.5" hidden="1" customHeight="1">
-      <c r="A79" s="249"/>
+      <c r="A79" s="232"/>
       <c r="B79" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C79" s="257"/>
+      <c r="C79" s="291"/>
       <c r="D79" s="47"/>
       <c r="E79" s="24"/>
       <c r="F79" s="24"/>
       <c r="G79" s="193"/>
-      <c r="H79" s="257"/>
+      <c r="H79" s="291"/>
       <c r="I79" s="194"/>
       <c r="J79" s="76"/>
       <c r="K79" s="6"/>
@@ -8753,24 +8713,24 @@
       <c r="AB79" s="3"/>
     </row>
     <row r="80" spans="1:28" ht="58.5" customHeight="1" thickBot="1">
-      <c r="A80" s="249"/>
+      <c r="A80" s="232"/>
       <c r="B80" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C80" s="258"/>
-      <c r="D80" s="234" t="s">
-        <v>101</v>
-      </c>
-      <c r="E80" s="227"/>
-      <c r="F80" s="272" t="s">
-        <v>124</v>
-      </c>
-      <c r="G80" s="264"/>
-      <c r="H80" s="257"/>
-      <c r="I80" s="234" t="s">
+      <c r="C80" s="292"/>
+      <c r="D80" s="268" t="s">
+        <v>100</v>
+      </c>
+      <c r="E80" s="256"/>
+      <c r="F80" s="317" t="s">
+        <v>123</v>
+      </c>
+      <c r="G80" s="243"/>
+      <c r="H80" s="291"/>
+      <c r="I80" s="268" t="s">
         <v>86</v>
       </c>
-      <c r="J80" s="221"/>
+      <c r="J80" s="247"/>
       <c r="K80" s="6"/>
       <c r="L80" s="2"/>
       <c r="M80" s="2"/>
@@ -8791,26 +8751,26 @@
       <c r="AB80" s="3"/>
     </row>
     <row r="81" spans="1:28" ht="50.25" thickBot="1">
-      <c r="A81" s="249"/>
+      <c r="A81" s="232"/>
       <c r="B81" s="18" t="s">
         <v>25</v>
       </c>
       <c r="C81" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="D81" s="273" t="s">
+      <c r="D81" s="318" t="s">
+        <v>105</v>
+      </c>
+      <c r="E81" s="282"/>
+      <c r="F81" s="255" t="s">
         <v>106</v>
       </c>
-      <c r="E81" s="274"/>
-      <c r="F81" s="224" t="s">
-        <v>107</v>
-      </c>
-      <c r="G81" s="264"/>
-      <c r="H81" s="257"/>
-      <c r="I81" s="269" t="s">
-        <v>211</v>
-      </c>
-      <c r="J81" s="221"/>
+      <c r="G81" s="243"/>
+      <c r="H81" s="291"/>
+      <c r="I81" s="342" t="s">
+        <v>210</v>
+      </c>
+      <c r="J81" s="247"/>
       <c r="K81" s="6"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
@@ -8831,26 +8791,26 @@
       <c r="AB81" s="3"/>
     </row>
     <row r="82" spans="1:28" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A82" s="250"/>
+      <c r="A82" s="233"/>
       <c r="B82" s="77" t="s">
         <v>26</v>
       </c>
       <c r="C82" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="D82" s="275" t="s">
+      <c r="D82" s="240" t="s">
+        <v>108</v>
+      </c>
+      <c r="E82" s="241"/>
+      <c r="F82" s="240" t="s">
         <v>109</v>
       </c>
-      <c r="E82" s="276"/>
-      <c r="F82" s="275" t="s">
-        <v>110</v>
-      </c>
-      <c r="G82" s="277"/>
-      <c r="H82" s="258"/>
-      <c r="I82" s="270" t="s">
-        <v>108</v>
-      </c>
-      <c r="J82" s="271"/>
+      <c r="G82" s="319"/>
+      <c r="H82" s="292"/>
+      <c r="I82" s="343" t="s">
+        <v>107</v>
+      </c>
+      <c r="J82" s="344"/>
       <c r="K82" s="6"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
@@ -8872,10 +8832,10 @@
     </row>
     <row r="83" spans="1:28" ht="20.25" thickBot="1">
       <c r="A83" s="196"/>
-      <c r="B83" s="346" t="s">
+      <c r="B83" s="220" t="s">
         <v>47</v>
       </c>
-      <c r="C83" s="347"/>
+      <c r="C83" s="221"/>
       <c r="D83" s="197"/>
       <c r="E83" s="198"/>
       <c r="F83" s="198"/>
@@ -8903,7 +8863,7 @@
       <c r="AB83" s="3"/>
     </row>
     <row r="84" spans="1:28" ht="20.25" thickBot="1">
-      <c r="A84" s="348" t="s">
+      <c r="A84" s="222" t="s">
         <v>47</v>
       </c>
       <c r="B84" s="200" t="s">
@@ -8911,16 +8871,16 @@
       </c>
       <c r="C84" s="200"/>
       <c r="D84" s="201" t="s">
+        <v>258</v>
+      </c>
+      <c r="E84" s="202" t="s">
         <v>259</v>
       </c>
-      <c r="E84" s="202" t="s">
+      <c r="F84" s="203" t="s">
         <v>260</v>
       </c>
-      <c r="F84" s="203" t="s">
+      <c r="G84" s="125" t="s">
         <v>261</v>
-      </c>
-      <c r="G84" s="125" t="s">
-        <v>262</v>
       </c>
       <c r="H84" s="204"/>
       <c r="I84" s="204"/>
@@ -8945,16 +8905,16 @@
       <c r="AB84" s="3"/>
     </row>
     <row r="85" spans="1:28" ht="66">
-      <c r="A85" s="349"/>
+      <c r="A85" s="223"/>
       <c r="B85" s="206" t="s">
         <v>15</v>
       </c>
-      <c r="C85" s="351"/>
+      <c r="C85" s="225"/>
       <c r="D85" s="107" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E85" s="108" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F85" s="171"/>
       <c r="G85" s="120"/>
@@ -8981,16 +8941,16 @@
       <c r="AB85" s="3"/>
     </row>
     <row r="86" spans="1:28" ht="66">
-      <c r="A86" s="349"/>
+      <c r="A86" s="223"/>
       <c r="B86" s="206" t="s">
         <v>17</v>
       </c>
-      <c r="C86" s="352"/>
+      <c r="C86" s="226"/>
       <c r="D86" s="108" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E86" s="107" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F86" s="171"/>
       <c r="G86" s="120"/>
@@ -9017,16 +8977,16 @@
       <c r="AB86" s="3"/>
     </row>
     <row r="87" spans="1:28" ht="49.5">
-      <c r="A87" s="349"/>
+      <c r="A87" s="223"/>
       <c r="B87" s="206" t="s">
         <v>18</v>
       </c>
-      <c r="C87" s="352"/>
+      <c r="C87" s="226"/>
       <c r="D87" s="108" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E87" s="187" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F87" s="171"/>
       <c r="G87" s="120"/>
@@ -9053,16 +9013,16 @@
       <c r="AB87" s="3"/>
     </row>
     <row r="88" spans="1:28" ht="66">
-      <c r="A88" s="349"/>
+      <c r="A88" s="223"/>
       <c r="B88" s="206" t="s">
         <v>19</v>
       </c>
-      <c r="C88" s="352"/>
+      <c r="C88" s="226"/>
       <c r="D88" s="187" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E88" s="108" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F88" s="172"/>
       <c r="G88" s="120"/>
@@ -9089,19 +9049,19 @@
       <c r="AB88" s="3"/>
     </row>
     <row r="89" spans="1:28" ht="49.5">
-      <c r="A89" s="349"/>
+      <c r="A89" s="223"/>
       <c r="B89" s="206" t="s">
         <v>21</v>
       </c>
-      <c r="C89" s="352"/>
+      <c r="C89" s="226"/>
       <c r="D89" s="108" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E89" s="108" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F89" s="173" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G89" s="120"/>
       <c r="H89" s="195"/>
@@ -9127,20 +9087,20 @@
       <c r="AB89" s="3"/>
     </row>
     <row r="90" spans="1:28" ht="50.25" thickBot="1">
-      <c r="A90" s="349"/>
+      <c r="A90" s="223"/>
       <c r="B90" s="212" t="s">
         <v>23</v>
       </c>
       <c r="C90" s="213"/>
       <c r="D90" s="181"/>
       <c r="E90" s="175" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F90" s="175" t="s">
+        <v>263</v>
+      </c>
+      <c r="G90" s="175" t="s">
         <v>264</v>
-      </c>
-      <c r="G90" s="175" t="s">
-        <v>265</v>
       </c>
       <c r="H90" s="195"/>
       <c r="I90" s="195"/>
@@ -9165,7 +9125,7 @@
       <c r="AB90" s="3"/>
     </row>
     <row r="91" spans="1:28" ht="32.25" thickBot="1">
-      <c r="A91" s="350"/>
+      <c r="A91" s="224"/>
       <c r="B91" s="212" t="s">
         <v>24</v>
       </c>
@@ -9174,8 +9134,8 @@
       <c r="E91" s="215"/>
       <c r="F91" s="215"/>
       <c r="G91" s="215"/>
-      <c r="H91" s="353"/>
-      <c r="I91" s="354"/>
+      <c r="H91" s="227"/>
+      <c r="I91" s="228"/>
       <c r="J91" s="216"/>
       <c r="K91" s="1"/>
       <c r="L91" s="2"/>
@@ -9198,10 +9158,10 @@
     </row>
     <row r="92" spans="1:28" ht="20.25" thickBot="1">
       <c r="A92" s="196"/>
-      <c r="B92" s="346" t="s">
+      <c r="B92" s="220" t="s">
         <v>54</v>
       </c>
-      <c r="C92" s="347"/>
+      <c r="C92" s="221"/>
       <c r="D92" s="197"/>
       <c r="E92" s="198"/>
       <c r="F92" s="198"/>
@@ -9229,7 +9189,7 @@
       <c r="AB92" s="3"/>
     </row>
     <row r="93" spans="1:28" ht="20.25" thickBot="1">
-      <c r="A93" s="348" t="s">
+      <c r="A93" s="222" t="s">
         <v>54</v>
       </c>
       <c r="B93" s="200" t="s">
@@ -9237,13 +9197,13 @@
       </c>
       <c r="C93" s="200"/>
       <c r="D93" s="201" t="s">
+        <v>258</v>
+      </c>
+      <c r="E93" s="202" t="s">
         <v>259</v>
       </c>
-      <c r="E93" s="202" t="s">
+      <c r="F93" s="203" t="s">
         <v>260</v>
-      </c>
-      <c r="F93" s="203" t="s">
-        <v>261</v>
       </c>
       <c r="G93" s="217"/>
       <c r="H93" s="204"/>
@@ -9269,16 +9229,16 @@
       <c r="AB93" s="3"/>
     </row>
     <row r="94" spans="1:28" ht="66">
-      <c r="A94" s="349"/>
+      <c r="A94" s="223"/>
       <c r="B94" s="206" t="s">
         <v>15</v>
       </c>
-      <c r="C94" s="351"/>
+      <c r="C94" s="225"/>
       <c r="D94" s="115" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E94" s="116" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F94" s="182"/>
       <c r="G94" s="218"/>
@@ -9305,16 +9265,16 @@
       <c r="AB94" s="3"/>
     </row>
     <row r="95" spans="1:28" ht="66">
-      <c r="A95" s="349"/>
+      <c r="A95" s="223"/>
       <c r="B95" s="206" t="s">
         <v>17</v>
       </c>
-      <c r="C95" s="352"/>
+      <c r="C95" s="226"/>
       <c r="D95" s="108" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E95" s="107" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F95" s="120"/>
       <c r="G95" s="207"/>
@@ -9341,19 +9301,19 @@
       <c r="AB95" s="3"/>
     </row>
     <row r="96" spans="1:28" ht="49.5">
-      <c r="A96" s="349"/>
+      <c r="A96" s="223"/>
       <c r="B96" s="206" t="s">
         <v>18</v>
       </c>
-      <c r="C96" s="352"/>
+      <c r="C96" s="226"/>
       <c r="D96" s="108" t="s">
+        <v>242</v>
+      </c>
+      <c r="E96" s="108" t="s">
         <v>243</v>
       </c>
-      <c r="E96" s="108" t="s">
-        <v>244</v>
-      </c>
       <c r="F96" s="108" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G96" s="207"/>
       <c r="H96" s="23"/>
@@ -9379,16 +9339,16 @@
       <c r="AB96" s="3"/>
     </row>
     <row r="97" spans="1:28" ht="49.5">
-      <c r="A97" s="349"/>
+      <c r="A97" s="223"/>
       <c r="B97" s="206" t="s">
         <v>19</v>
       </c>
-      <c r="C97" s="352"/>
+      <c r="C97" s="226"/>
       <c r="D97" s="108" t="s">
+        <v>119</v>
+      </c>
+      <c r="E97" s="108" t="s">
         <v>120</v>
-      </c>
-      <c r="E97" s="108" t="s">
-        <v>121</v>
       </c>
       <c r="F97" s="171"/>
       <c r="G97" s="31"/>
@@ -9415,22 +9375,22 @@
       <c r="AB97" s="3"/>
     </row>
     <row r="98" spans="1:28" ht="66.75" thickBot="1">
-      <c r="A98" s="349"/>
+      <c r="A98" s="223"/>
       <c r="B98" s="206" t="s">
         <v>21</v>
       </c>
-      <c r="C98" s="352"/>
+      <c r="C98" s="226"/>
       <c r="D98" s="169" t="s">
+        <v>266</v>
+      </c>
+      <c r="E98" s="169" t="s">
         <v>267</v>
-      </c>
-      <c r="E98" s="169" t="s">
-        <v>268</v>
       </c>
       <c r="F98" s="185"/>
       <c r="G98" s="219"/>
       <c r="H98" s="195"/>
-      <c r="I98" s="228"/>
-      <c r="J98" s="355"/>
+      <c r="I98" s="229"/>
+      <c r="J98" s="230"/>
       <c r="K98" s="1"/>
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
@@ -9452,8 +9412,8 @@
     </row>
     <row r="99" spans="1:28" ht="19.5">
       <c r="A99" s="196"/>
-      <c r="B99" s="346"/>
-      <c r="C99" s="347"/>
+      <c r="B99" s="220"/>
+      <c r="C99" s="221"/>
       <c r="D99" s="197"/>
       <c r="E99" s="198"/>
       <c r="F99" s="198"/>
@@ -36482,15 +36442,127 @@
     </row>
   </sheetData>
   <mergeCells count="154">
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="A84:A91"/>
-    <mergeCell ref="C85:C89"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="A93:A98"/>
-    <mergeCell ref="C94:C98"/>
-    <mergeCell ref="I98:J98"/>
-    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A68:A82"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="C72:C80"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H69:H82"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="I80:J80"/>
+    <mergeCell ref="I81:J81"/>
+    <mergeCell ref="I82:J82"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="C41:C49"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="I56:J56"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="A37:A51"/>
+    <mergeCell ref="A53:A66"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="G1:J2"/>
+    <mergeCell ref="A2:E4"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C10:C20"/>
+    <mergeCell ref="A7:A20"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="A22:A35"/>
     <mergeCell ref="C26:C33"/>
     <mergeCell ref="D35:E35"/>
@@ -36515,127 +36587,15 @@
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="H31:I31"/>
     <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="G1:J2"/>
-    <mergeCell ref="A2:E4"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="C10:C20"/>
-    <mergeCell ref="A7:A20"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F78:G78"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="I56:J56"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="A37:A51"/>
-    <mergeCell ref="A53:A66"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="C41:C49"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="A68:A82"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C57:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="C72:C80"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H69:H82"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="I78:J78"/>
-    <mergeCell ref="I80:J80"/>
-    <mergeCell ref="I81:J81"/>
-    <mergeCell ref="I82:J82"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="I61:J61"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="A84:A91"/>
+    <mergeCell ref="C85:C89"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="A93:A98"/>
+    <mergeCell ref="C94:C98"/>
+    <mergeCell ref="I98:J98"/>
+    <mergeCell ref="B99:C99"/>
   </mergeCells>
   <pageMargins left="0.216187305364964" right="0.14099172089019399" top="0.26" bottom="0.25" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="25" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -36662,7 +36622,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
       <c r="A1" s="356" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B1" s="357"/>
       <c r="C1" s="357"/>
@@ -36688,16 +36648,16 @@
       <c r="A3" s="357"/>
       <c r="B3" s="357"/>
       <c r="C3" s="105" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3" s="105" t="s">
         <v>245</v>
       </c>
-      <c r="D3" s="105" t="s">
+      <c r="E3" s="105" t="s">
         <v>246</v>
       </c>
-      <c r="E3" s="105" t="s">
+      <c r="F3" s="105" t="s">
         <v>247</v>
-      </c>
-      <c r="F3" s="105" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="66">
@@ -36708,10 +36668,10 @@
         <v>48</v>
       </c>
       <c r="C4" s="107" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D4" s="108" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" s="171"/>
       <c r="F4" s="120"/>
@@ -36724,10 +36684,10 @@
         <v>49</v>
       </c>
       <c r="C5" s="108" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="107" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E5" s="171"/>
       <c r="F5" s="120"/>
@@ -36740,10 +36700,10 @@
         <v>50</v>
       </c>
       <c r="C6" s="108" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D6" s="187" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E6" s="171"/>
       <c r="F6" s="120"/>
@@ -36756,10 +36716,10 @@
         <v>51</v>
       </c>
       <c r="C7" s="187" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D7" s="108" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E7" s="172"/>
       <c r="F7" s="120"/>
@@ -36772,13 +36732,13 @@
         <v>53</v>
       </c>
       <c r="C8" s="108" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D8" s="108" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E8" s="173" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F8" s="120"/>
     </row>
@@ -36787,17 +36747,17 @@
         <v>52</v>
       </c>
       <c r="B9" s="112" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C9" s="181"/>
       <c r="D9" s="175" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E9" s="175" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F9" s="175" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="66">
@@ -36808,10 +36768,10 @@
         <v>48</v>
       </c>
       <c r="C10" s="115" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D10" s="116" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E10" s="182"/>
       <c r="F10" s="183"/>
@@ -36824,10 +36784,10 @@
         <v>49</v>
       </c>
       <c r="C11" s="108" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="107" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E11" s="120"/>
       <c r="F11" s="184"/>
@@ -36840,13 +36800,13 @@
         <v>50</v>
       </c>
       <c r="C12" s="108" t="s">
+        <v>242</v>
+      </c>
+      <c r="D12" s="108" t="s">
         <v>243</v>
       </c>
-      <c r="D12" s="108" t="s">
-        <v>244</v>
-      </c>
       <c r="E12" s="108" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F12" s="184"/>
     </row>
@@ -36858,10 +36818,10 @@
         <v>51</v>
       </c>
       <c r="C13" s="108" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="108" t="s">
         <v>120</v>
-      </c>
-      <c r="D13" s="108" t="s">
-        <v>121</v>
       </c>
       <c r="E13" s="171"/>
       <c r="F13" s="184"/>
@@ -36874,10 +36834,10 @@
         <v>53</v>
       </c>
       <c r="C14" s="169" t="s">
+        <v>266</v>
+      </c>
+      <c r="D14" s="169" t="s">
         <v>267</v>
-      </c>
-      <c r="D14" s="169" t="s">
-        <v>268</v>
       </c>
       <c r="E14" s="185"/>
       <c r="F14" s="186"/>

</xml_diff>